<commit_message>
final edit done ready to deploy
</commit_message>
<xml_diff>
--- a/data/carl_demo_requests.xlsx
+++ b/data/carl_demo_requests.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -953,16 +953,11 @@
           <t>Diksha</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>diksha@iengaust.com.au</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
           <t>Requested: Australia User Manual Revision</t>
@@ -971,6 +966,54 @@
       <c r="J13" t="inlineStr">
         <is>
           <t>192.168.1.68</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-16 02:31:30 UTC</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sujay jirapure</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>KGN Solar</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>jirapuresujay@gmail.com</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>+91</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>+9161408591185</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>50 Broughton Road</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>192.168.1.54</t>
         </is>
       </c>
     </row>

</xml_diff>